<commit_message>
specify location of injury
</commit_message>
<xml_diff>
--- a/storage/FWRI1.xlsx
+++ b/storage/FWRI1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cesu\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC66E269-A549-40F3-919E-20B0D362837B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AFE0E4-4D57-44BC-BDFA-833732A7A8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{76154FC2-4AB5-4F8C-9B6F-69F6CFB7390F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Injury Registry Form: Fax (046) 416-4942, SMS : 09284895496, email address: pesucavite@gmail.com</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Aware of Any Health Education Materials Regarding Fireworks</t>
+  </si>
+  <si>
+    <t>Specify Location of Injury</t>
   </si>
 </sst>
 </file>
@@ -331,9 +334,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -342,12 +342,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -390,6 +384,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -705,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E2AB8A-9591-4B95-8FE2-C7938384E68B}">
-  <dimension ref="B1:U104"/>
+  <dimension ref="B1:V104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,207 +721,216 @@
     <col min="4" max="4" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="8" width="54.42578125" customWidth="1"/>
-    <col min="9" max="12" width="42.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" customWidth="1"/>
-    <col min="20" max="20" width="26.5703125" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="42.7109375" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
+    <col min="15" max="15" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" customWidth="1"/>
+    <col min="21" max="21" width="26.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D1" s="19" t="s">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-    </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D2" s="19" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D3" s="20" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-    </row>
-    <row r="5" spans="2:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+    </row>
+    <row r="5" spans="2:22" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="N5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="O5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="P5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="Q5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="R5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="S5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="T5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="U5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="V5" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -939,8 +951,9 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V8" s="1"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -961,8 +974,9 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V9" s="1"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -983,8 +997,9 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V10" s="1"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1005,8 +1020,9 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V11" s="1"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1027,8 +1043,9 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V12" s="1"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1049,8 +1066,9 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1071,8 +1089,9 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1093,8 +1112,9 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1115,8 +1135,9 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1137,8 +1158,9 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1159,8 +1181,9 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1181,8 +1204,9 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1203,8 +1227,9 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1225,8 +1250,9 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1247,8 +1273,9 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1269,8 +1296,9 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1291,8 +1319,9 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1313,8 +1342,9 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="1"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1335,8 +1365,9 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V26" s="1"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1357,8 +1388,9 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V27" s="1"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1379,8 +1411,9 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1401,8 +1434,9 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="1"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1423,8 +1457,9 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V30" s="1"/>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1445,8 +1480,9 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V31" s="1"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1467,8 +1503,9 @@
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V32" s="1"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1489,8 +1526,9 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V33" s="1"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1511,8 +1549,9 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V34" s="1"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1533,8 +1572,9 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V35" s="1"/>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1555,8 +1595,9 @@
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1577,8 +1618,9 @@
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V37" s="1"/>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1599,8 +1641,9 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V38" s="1"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1621,8 +1664,9 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V39" s="1"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1643,8 +1687,9 @@
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
-    </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V40" s="1"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1665,8 +1710,9 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V41" s="1"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1687,8 +1733,9 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
-    </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V42" s="1"/>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1709,8 +1756,9 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
-    </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V43" s="1"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1731,8 +1779,9 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
-    </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V44" s="1"/>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1753,8 +1802,9 @@
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
-    </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V45" s="1"/>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1775,8 +1825,9 @@
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
-    </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V46" s="1"/>
+    </row>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1797,8 +1848,9 @@
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
-    </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V47" s="1"/>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1819,8 +1871,9 @@
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
-    </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V48" s="1"/>
+    </row>
+    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1841,8 +1894,9 @@
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
-    </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V49" s="1"/>
+    </row>
+    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1863,8 +1917,9 @@
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
-    </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V50" s="1"/>
+    </row>
+    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1885,8 +1940,9 @@
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
-    </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V51" s="1"/>
+    </row>
+    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1907,8 +1963,9 @@
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
-    </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V52" s="1"/>
+    </row>
+    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1929,8 +1986,9 @@
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
-    </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V53" s="1"/>
+    </row>
+    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1951,8 +2009,9 @@
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
-    </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V54" s="1"/>
+    </row>
+    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1973,8 +2032,9 @@
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
-    </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V55" s="1"/>
+    </row>
+    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1995,8 +2055,9 @@
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
-    </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V56" s="1"/>
+    </row>
+    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2017,8 +2078,9 @@
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
-    </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V57" s="1"/>
+    </row>
+    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2039,8 +2101,9 @@
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
-    </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V58" s="1"/>
+    </row>
+    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -2061,8 +2124,9 @@
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
-    </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V59" s="1"/>
+    </row>
+    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -2083,8 +2147,9 @@
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
-    </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V60" s="1"/>
+    </row>
+    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -2105,8 +2170,9 @@
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
-    </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V61" s="1"/>
+    </row>
+    <row r="62" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2127,8 +2193,9 @@
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
-    </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V62" s="1"/>
+    </row>
+    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2149,8 +2216,9 @@
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
-    </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V63" s="1"/>
+    </row>
+    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2171,8 +2239,9 @@
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
-    </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V64" s="1"/>
+    </row>
+    <row r="65" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2193,8 +2262,9 @@
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
-    </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V65" s="1"/>
+    </row>
+    <row r="66" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2215,8 +2285,9 @@
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
-    </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V66" s="1"/>
+    </row>
+    <row r="67" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2237,8 +2308,9 @@
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
-    </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V67" s="1"/>
+    </row>
+    <row r="68" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2259,8 +2331,9 @@
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
-    </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V68" s="1"/>
+    </row>
+    <row r="69" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2281,8 +2354,9 @@
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
-    </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V69" s="1"/>
+    </row>
+    <row r="70" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2303,8 +2377,9 @@
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
-    </row>
-    <row r="71" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V70" s="1"/>
+    </row>
+    <row r="71" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -2325,8 +2400,9 @@
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
-    </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V71" s="1"/>
+    </row>
+    <row r="72" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -2347,8 +2423,9 @@
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
-    </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V72" s="1"/>
+    </row>
+    <row r="73" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2369,8 +2446,9 @@
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
-    </row>
-    <row r="74" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V73" s="1"/>
+    </row>
+    <row r="74" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2391,8 +2469,9 @@
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
-    </row>
-    <row r="75" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V74" s="1"/>
+    </row>
+    <row r="75" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2413,8 +2492,9 @@
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
-    </row>
-    <row r="76" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V75" s="1"/>
+    </row>
+    <row r="76" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2435,8 +2515,9 @@
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
-    </row>
-    <row r="77" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V76" s="1"/>
+    </row>
+    <row r="77" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2457,8 +2538,9 @@
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
-    </row>
-    <row r="78" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V77" s="1"/>
+    </row>
+    <row r="78" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2479,8 +2561,9 @@
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
-    </row>
-    <row r="79" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V78" s="1"/>
+    </row>
+    <row r="79" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2501,8 +2584,9 @@
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
-    </row>
-    <row r="80" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V79" s="1"/>
+    </row>
+    <row r="80" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2523,8 +2607,9 @@
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
-    </row>
-    <row r="81" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V80" s="1"/>
+    </row>
+    <row r="81" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2545,8 +2630,9 @@
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
-    </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V81" s="1"/>
+    </row>
+    <row r="82" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2567,8 +2653,9 @@
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
-    </row>
-    <row r="83" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V82" s="1"/>
+    </row>
+    <row r="83" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2589,8 +2676,9 @@
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
-    </row>
-    <row r="84" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V83" s="1"/>
+    </row>
+    <row r="84" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2611,8 +2699,9 @@
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
-    </row>
-    <row r="85" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V84" s="1"/>
+    </row>
+    <row r="85" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2633,8 +2722,9 @@
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
-    </row>
-    <row r="86" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V85" s="1"/>
+    </row>
+    <row r="86" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -2655,8 +2745,9 @@
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
-    </row>
-    <row r="87" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V86" s="1"/>
+    </row>
+    <row r="87" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -2677,8 +2768,9 @@
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
-    </row>
-    <row r="88" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V87" s="1"/>
+    </row>
+    <row r="88" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -2699,8 +2791,9 @@
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
-    </row>
-    <row r="89" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V88" s="1"/>
+    </row>
+    <row r="89" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -2721,8 +2814,9 @@
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
-    </row>
-    <row r="90" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V89" s="1"/>
+    </row>
+    <row r="90" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -2743,8 +2837,9 @@
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
-    </row>
-    <row r="91" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V90" s="1"/>
+    </row>
+    <row r="91" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -2765,8 +2860,9 @@
       <c r="S91" s="1"/>
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
-    </row>
-    <row r="92" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V91" s="1"/>
+    </row>
+    <row r="92" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -2787,8 +2883,9 @@
       <c r="S92" s="1"/>
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
-    </row>
-    <row r="93" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V92" s="1"/>
+    </row>
+    <row r="93" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -2809,8 +2906,9 @@
       <c r="S93" s="1"/>
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
-    </row>
-    <row r="94" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V93" s="1"/>
+    </row>
+    <row r="94" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -2831,8 +2929,9 @@
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
-    </row>
-    <row r="95" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V94" s="1"/>
+    </row>
+    <row r="95" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -2853,8 +2952,9 @@
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
-    </row>
-    <row r="96" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V95" s="1"/>
+    </row>
+    <row r="96" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -2875,8 +2975,9 @@
       <c r="S96" s="1"/>
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
-    </row>
-    <row r="97" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V96" s="1"/>
+    </row>
+    <row r="97" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -2897,8 +2998,9 @@
       <c r="S97" s="1"/>
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
-    </row>
-    <row r="98" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V97" s="1"/>
+    </row>
+    <row r="98" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -2919,8 +3021,9 @@
       <c r="S98" s="1"/>
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
-    </row>
-    <row r="99" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V98" s="1"/>
+    </row>
+    <row r="99" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -2941,8 +3044,9 @@
       <c r="S99" s="1"/>
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
-    </row>
-    <row r="100" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V99" s="1"/>
+    </row>
+    <row r="100" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -2963,8 +3067,9 @@
       <c r="S100" s="1"/>
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
-    </row>
-    <row r="101" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V100" s="1"/>
+    </row>
+    <row r="101" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -2985,129 +3090,134 @@
       <c r="S101" s="1"/>
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
-    </row>
-    <row r="102" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="V101" s="1"/>
+    </row>
+    <row r="102" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D102" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E102" s="28" t="s">
+      <c r="E102" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F102" s="29"/>
+      <c r="F102" s="26"/>
       <c r="G102" s="8"/>
       <c r="H102" s="8"/>
-      <c r="I102" s="21" t="s">
+      <c r="I102" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J102" s="21"/>
-      <c r="K102" s="21"/>
-      <c r="L102" s="21"/>
-      <c r="M102" s="21"/>
-      <c r="N102" s="23" t="s">
+      <c r="J102" s="18"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="18"/>
+      <c r="M102" s="18"/>
+      <c r="N102" s="18"/>
+      <c r="O102" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O102" s="23"/>
-      <c r="P102" s="23"/>
-      <c r="Q102" s="5"/>
-      <c r="R102" s="21" t="s">
+      <c r="P102" s="20"/>
+      <c r="Q102" s="20"/>
+      <c r="R102" s="5"/>
+      <c r="S102" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="S102" s="21"/>
-      <c r="T102" s="21"/>
-    </row>
-    <row r="103" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T102" s="18"/>
+      <c r="U102" s="18"/>
+    </row>
+    <row r="103" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D103" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E103" s="26" t="s">
+      <c r="E103" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F103" s="27"/>
+      <c r="F103" s="24"/>
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
-      <c r="I103" s="24" t="s">
+      <c r="I103" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J103" s="24"/>
-      <c r="K103" s="24"/>
-      <c r="L103" s="24"/>
-      <c r="M103" s="24"/>
-      <c r="N103" s="24" t="s">
+      <c r="J103" s="21"/>
+      <c r="K103" s="21"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="21"/>
+      <c r="N103" s="21"/>
+      <c r="O103" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="O103" s="24"/>
-      <c r="P103" s="24"/>
-      <c r="Q103" s="6"/>
-      <c r="R103" s="22" t="s">
+      <c r="P103" s="21"/>
+      <c r="Q103" s="21"/>
+      <c r="R103" s="6"/>
+      <c r="S103" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="S103" s="22"/>
-      <c r="T103" s="22"/>
-    </row>
-    <row r="104" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T103" s="19"/>
+      <c r="U103" s="19"/>
+    </row>
+    <row r="104" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D104" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E104" s="14" t="s">
+      <c r="E104" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F104" s="15"/>
+      <c r="F104" s="29"/>
       <c r="G104" s="9"/>
       <c r="H104" s="9"/>
-      <c r="I104" s="25" t="s">
+      <c r="I104" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J104" s="25"/>
-      <c r="K104" s="25"/>
-      <c r="L104" s="25"/>
-      <c r="M104" s="25"/>
-      <c r="N104" s="22" t="s">
+      <c r="J104" s="22"/>
+      <c r="K104" s="22"/>
+      <c r="L104" s="22"/>
+      <c r="M104" s="22"/>
+      <c r="N104" s="22"/>
+      <c r="O104" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="O104" s="22"/>
-      <c r="P104" s="22"/>
-      <c r="Q104" s="4"/>
-      <c r="R104" s="22"/>
-      <c r="S104" s="22"/>
-      <c r="T104" s="22"/>
+      <c r="P104" s="19"/>
+      <c r="Q104" s="19"/>
+      <c r="R104" s="4"/>
+      <c r="S104" s="19"/>
+      <c r="T104" s="19"/>
+      <c r="U104" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="36">
+    <mergeCell ref="D4:U4"/>
+    <mergeCell ref="T5:T7"/>
     <mergeCell ref="U5:U7"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="R5:R7"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="D1:U1"/>
+    <mergeCell ref="D2:U2"/>
+    <mergeCell ref="D3:U3"/>
+    <mergeCell ref="S102:U102"/>
+    <mergeCell ref="S103:U104"/>
+    <mergeCell ref="O102:Q102"/>
+    <mergeCell ref="O103:Q103"/>
+    <mergeCell ref="O104:Q104"/>
+    <mergeCell ref="I102:N102"/>
+    <mergeCell ref="I103:N103"/>
+    <mergeCell ref="I104:N104"/>
+    <mergeCell ref="E103:F103"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="S5:S7"/>
+    <mergeCell ref="V5:V7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="J5:J7"/>
     <mergeCell ref="I5:I7"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D1:T1"/>
-    <mergeCell ref="D2:T2"/>
-    <mergeCell ref="D3:T3"/>
-    <mergeCell ref="R102:T102"/>
-    <mergeCell ref="R103:T104"/>
-    <mergeCell ref="N102:P102"/>
-    <mergeCell ref="N103:P103"/>
-    <mergeCell ref="N104:P104"/>
-    <mergeCell ref="I102:M102"/>
-    <mergeCell ref="I103:M103"/>
-    <mergeCell ref="I104:M104"/>
-    <mergeCell ref="E103:F103"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="R5:R7"/>
-    <mergeCell ref="D4:T4"/>
-    <mergeCell ref="S5:S7"/>
-    <mergeCell ref="T5:T7"/>
-    <mergeCell ref="E104:F104"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="Q5:Q7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>